<commit_message>
Final code push in to GIT
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Master_Sheet.xlsx
+++ b/src/test/resources/testData/Master_Sheet.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BYMAT-Learn_Automation\WorkSpace\WorkSpace_Photon\SeleniumTraining_B9_MVN\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9908E9C6-9C08-4281-B2E6-544B3737F7FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16BCD199-30BD-45FB-8530-12A5008EE53B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Test_Data" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="TestCases" sheetId="2" r:id="rId1"/>
+    <sheet name="Test_Data" sheetId="1" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TestCases!$A$1:$E$7</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="37">
   <si>
     <t>Sr.No</t>
   </si>
@@ -61,12 +64,6 @@
     <t>CREATE AN ACCOUNT</t>
   </si>
   <si>
-    <t>loginToMyStore</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>Deepali</t>
   </si>
   <si>
@@ -79,9 +76,6 @@
     <t>Deepali@gmail.com</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
     <t>Lipika</t>
   </si>
   <si>
@@ -134,13 +128,25 @@
   </si>
   <si>
     <t>My St</t>
+  </si>
+  <si>
+    <t>TestCase_Name</t>
+  </si>
+  <si>
+    <t>Run_Mode</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,6 +158,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -199,13 +213,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -486,11 +506,114 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7222312-3CDF-431F-ABBE-B25F48B8310F}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="5.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="7">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="7">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:E7" xr:uid="{F7222312-3CDF-431F-ABBE-B25F48B8310F}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -506,7 +629,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B1" s="5"/>
     </row>
@@ -538,16 +661,16 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>16</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>8</v>
@@ -558,7 +681,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B5" s="5"/>
     </row>
@@ -590,16 +713,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>8</v>
@@ -610,7 +733,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B9" s="5"/>
     </row>
@@ -642,16 +765,16 @@
         <v>6</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>8</v>
@@ -662,7 +785,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B13" s="5"/>
     </row>
@@ -694,16 +817,16 @@
         <v>6</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>8</v>
@@ -714,7 +837,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B17" s="5"/>
     </row>
@@ -746,19 +869,19 @@
         <v>6</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>10</v>
@@ -766,7 +889,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B21" s="5"/>
     </row>
@@ -798,16 +921,16 @@
         <v>6</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>8</v>
@@ -827,130 +950,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7222312-3CDF-431F-ABBE-B25F48B8310F}">
-  <dimension ref="A1:G5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="5.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="5"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" xr:uid="{8CAB58FF-08E2-4A76-AD4C-5781CB0A7922}"/>
-    <hyperlink ref="E4" r:id="rId2" xr:uid="{952BD0E7-9ADF-4354-8876-A42FEB218BBF}"/>
-    <hyperlink ref="E5" r:id="rId3" xr:uid="{E7C494AB-68C7-4CB8-AB43-A2F3A5A6C127}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Check in SC to verify if Jenkins trigger a build
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Master_Sheet.xlsx
+++ b/src/test/resources/testData/Master_Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BYMAT-Learn_Automation\WorkSpace\WorkSpace_Photon\SeleniumTraining_B9_MVN\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16BCD199-30BD-45FB-8530-12A5008EE53B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BDF133A-EC87-4B5C-9B42-746C5CC892FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="36">
   <si>
     <t>Sr.No</t>
   </si>
@@ -125,9 +125,6 @@
   </si>
   <si>
     <t>MadarTC6</t>
-  </si>
-  <si>
-    <t>My St</t>
   </si>
   <si>
     <t>TestCase_Name</t>
@@ -509,7 +506,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7222312-3CDF-431F-ABBE-B25F48B8310F}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -529,10 +526,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -543,7 +540,7 @@
         <v>23</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -554,7 +551,7 @@
         <v>21</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -565,7 +562,7 @@
         <v>22</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -576,7 +573,7 @@
         <v>24</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -587,7 +584,7 @@
         <v>28</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -598,7 +595,7 @@
         <v>29</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -612,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -881,7 +878,7 @@
         <v>20</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>10</v>

</xml_diff>